<commit_message>
Added Schluter et al. 2004
</commit_message>
<xml_diff>
--- a/data/pigment_mass_ratios.xlsx
+++ b/data/pigment_mass_ratios.xlsx
@@ -7,7 +7,7 @@
     <workbookView windowWidth="28800" windowHeight="12045"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -916,7 +916,7 @@
     <t>Zapata et al. 2004</t>
   </si>
   <si>
-    <t>Pavlovophytes</t>
+    <t>Prymnesiophytes</t>
   </si>
   <si>
     <t>Chrysotila</t>
@@ -931,13 +931,13 @@
     <t>HAPTO_12</t>
   </si>
   <si>
-    <t>Prymnesiophytes</t>
-  </si>
-  <si>
     <t>Chrysotila roscoffensis</t>
   </si>
   <si>
     <t>Pleurochrysis roscoffensis</t>
+  </si>
+  <si>
+    <t>Pavlovophytes</t>
   </si>
   <si>
     <t>Diacronema</t>
@@ -1194,11 +1194,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="0.000_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="0.000_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -1254,10 +1254,25 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1269,8 +1284,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1285,14 +1324,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1314,45 +1360,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1360,30 +1367,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1398,13 +1398,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1416,115 +1482,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1542,7 +1500,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1554,7 +1518,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1566,7 +1542,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1578,7 +1572,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1592,11 +1592,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1605,7 +1611,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1651,17 +1657,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1680,156 +1689,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1852,7 +1852,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
@@ -1870,22 +1870,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1894,7 +1894,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1903,10 +1903,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2236,7 +2236,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -57647,16 +57647,16 @@
         <v>299</v>
       </c>
       <c r="B266" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C266" s="7" t="s">
         <v>301</v>
       </c>
       <c r="D266" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="E266" s="7" t="s">
         <v>306</v>
-      </c>
-      <c r="E266" s="7" t="s">
-        <v>307</v>
       </c>
       <c r="F266" s="6">
         <v>1327470</v>
@@ -57856,7 +57856,7 @@
         <v>299</v>
       </c>
       <c r="B267" s="6" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="C267" s="7" t="s">
         <v>308</v>
@@ -58065,7 +58065,7 @@
         <v>299</v>
       </c>
       <c r="B268" s="6" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="C268" s="7" t="s">
         <v>308</v>
@@ -58274,7 +58274,7 @@
         <v>299</v>
       </c>
       <c r="B269" s="6" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="C269" s="7" t="s">
         <v>308</v>
@@ -58483,7 +58483,7 @@
         <v>299</v>
       </c>
       <c r="B270" s="6" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="C270" s="7" t="s">
         <v>308</v>
@@ -58692,7 +58692,7 @@
         <v>299</v>
       </c>
       <c r="B271" s="6" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="C271" s="7" t="s">
         <v>313</v>
@@ -58901,7 +58901,7 @@
         <v>299</v>
       </c>
       <c r="B272" s="6" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="C272" s="7" t="s">
         <v>313</v>
@@ -59110,7 +59110,7 @@
         <v>299</v>
       </c>
       <c r="B273" s="6" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="C273" s="7" t="s">
         <v>313</v>
@@ -59319,7 +59319,7 @@
         <v>299</v>
       </c>
       <c r="B274" s="6" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="C274" s="7" t="s">
         <v>313</v>
@@ -59528,7 +59528,7 @@
         <v>299</v>
       </c>
       <c r="B275" s="6" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="C275" s="7" t="s">
         <v>313</v>
@@ -59737,7 +59737,7 @@
         <v>299</v>
       </c>
       <c r="B276" s="6" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="C276" s="7" t="s">
         <v>313</v>
@@ -59946,7 +59946,7 @@
         <v>299</v>
       </c>
       <c r="B277" s="6" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="C277" s="7" t="s">
         <v>317</v>
@@ -60155,7 +60155,7 @@
         <v>299</v>
       </c>
       <c r="B278" s="6" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="C278" s="7" t="s">
         <v>320</v>
@@ -60364,7 +60364,7 @@
         <v>299</v>
       </c>
       <c r="B279" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C279" s="7" t="s">
         <v>301</v>
@@ -60573,7 +60573,7 @@
         <v>299</v>
       </c>
       <c r="B280" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C280" s="7" t="s">
         <v>325</v>
@@ -60782,7 +60782,7 @@
         <v>299</v>
       </c>
       <c r="B281" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C281" s="7" t="s">
         <v>325</v>
@@ -60991,7 +60991,7 @@
         <v>299</v>
       </c>
       <c r="B282" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C282" s="7" t="s">
         <v>327</v>
@@ -61200,7 +61200,7 @@
         <v>299</v>
       </c>
       <c r="B283" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C283" s="7" t="s">
         <v>327</v>
@@ -61409,7 +61409,7 @@
         <v>69</v>
       </c>
       <c r="B284" s="23" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C284" s="7" t="s">
         <v>327</v>
@@ -61618,7 +61618,7 @@
         <v>69</v>
       </c>
       <c r="B285" s="23" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C285" s="7" t="s">
         <v>327</v>
@@ -61827,7 +61827,7 @@
         <v>69</v>
       </c>
       <c r="B286" s="23" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C286" s="7" t="s">
         <v>327</v>
@@ -62036,7 +62036,7 @@
         <v>69</v>
       </c>
       <c r="B287" s="23" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C287" s="7" t="s">
         <v>327</v>
@@ -62245,7 +62245,7 @@
         <v>299</v>
       </c>
       <c r="B288" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C288" s="7" t="s">
         <v>327</v>
@@ -62454,7 +62454,7 @@
         <v>299</v>
       </c>
       <c r="B289" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C289" s="7" t="s">
         <v>330</v>
@@ -62663,7 +62663,7 @@
         <v>299</v>
       </c>
       <c r="B290" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C290" s="6" t="s">
         <v>75</v>
@@ -62872,7 +62872,7 @@
         <v>299</v>
       </c>
       <c r="B291" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C291" s="7" t="s">
         <v>334</v>
@@ -63081,7 +63081,7 @@
         <v>299</v>
       </c>
       <c r="B292" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C292" s="7" t="s">
         <v>334</v>
@@ -63290,7 +63290,7 @@
         <v>299</v>
       </c>
       <c r="B293" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C293" s="7" t="s">
         <v>334</v>
@@ -63499,7 +63499,7 @@
         <v>299</v>
       </c>
       <c r="B294" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C294" s="7" t="s">
         <v>334</v>
@@ -63708,7 +63708,7 @@
         <v>299</v>
       </c>
       <c r="B295" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C295" s="7" t="s">
         <v>334</v>
@@ -63917,7 +63917,7 @@
         <v>299</v>
       </c>
       <c r="B296" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C296" s="7" t="s">
         <v>339</v>
@@ -64126,7 +64126,7 @@
         <v>299</v>
       </c>
       <c r="B297" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C297" s="6" t="s">
         <v>75</v>
@@ -64335,7 +64335,7 @@
         <v>299</v>
       </c>
       <c r="B298" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C298" s="7" t="s">
         <v>344</v>
@@ -64544,7 +64544,7 @@
         <v>299</v>
       </c>
       <c r="B299" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C299" s="7" t="s">
         <v>346</v>
@@ -64753,7 +64753,7 @@
         <v>299</v>
       </c>
       <c r="B300" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C300" s="7" t="s">
         <v>346</v>
@@ -64962,7 +64962,7 @@
         <v>299</v>
       </c>
       <c r="B301" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C301" s="7" t="s">
         <v>346</v>
@@ -65171,7 +65171,7 @@
         <v>299</v>
       </c>
       <c r="B302" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C302" s="7" t="s">
         <v>346</v>
@@ -65380,7 +65380,7 @@
         <v>299</v>
       </c>
       <c r="B303" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C303" s="7" t="s">
         <v>346</v>
@@ -65589,7 +65589,7 @@
         <v>299</v>
       </c>
       <c r="B304" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C304" s="7" t="s">
         <v>346</v>
@@ -65798,7 +65798,7 @@
         <v>299</v>
       </c>
       <c r="B305" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C305" s="7" t="s">
         <v>346</v>
@@ -66007,7 +66007,7 @@
         <v>299</v>
       </c>
       <c r="B306" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C306" s="7" t="s">
         <v>346</v>
@@ -66216,7 +66216,7 @@
         <v>299</v>
       </c>
       <c r="B307" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C307" s="7" t="s">
         <v>346</v>
@@ -66425,7 +66425,7 @@
         <v>299</v>
       </c>
       <c r="B308" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C308" s="7" t="s">
         <v>346</v>
@@ -66634,7 +66634,7 @@
         <v>299</v>
       </c>
       <c r="B309" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C309" s="7" t="s">
         <v>346</v>
@@ -66843,7 +66843,7 @@
         <v>69</v>
       </c>
       <c r="B310" s="23" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C310" s="7" t="s">
         <v>346</v>
@@ -67052,7 +67052,7 @@
         <v>69</v>
       </c>
       <c r="B311" s="23" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C311" s="7" t="s">
         <v>346</v>
@@ -67261,7 +67261,7 @@
         <v>69</v>
       </c>
       <c r="B312" s="23" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C312" s="7" t="s">
         <v>346</v>
@@ -67470,7 +67470,7 @@
         <v>69</v>
       </c>
       <c r="B313" s="23" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C313" s="7" t="s">
         <v>346</v>
@@ -67679,7 +67679,7 @@
         <v>299</v>
       </c>
       <c r="B314" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C314" s="7" t="s">
         <v>349</v>
@@ -67888,7 +67888,7 @@
         <v>299</v>
       </c>
       <c r="B315" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C315" s="7" t="s">
         <v>351</v>
@@ -68097,7 +68097,7 @@
         <v>299</v>
       </c>
       <c r="B316" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C316" s="7" t="s">
         <v>351</v>
@@ -68306,7 +68306,7 @@
         <v>299</v>
       </c>
       <c r="B317" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C317" s="7" t="s">
         <v>351</v>
@@ -68515,7 +68515,7 @@
         <v>299</v>
       </c>
       <c r="B318" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C318" s="7" t="s">
         <v>356</v>
@@ -68724,7 +68724,7 @@
         <v>299</v>
       </c>
       <c r="B319" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C319" s="7" t="s">
         <v>356</v>
@@ -68933,7 +68933,7 @@
         <v>299</v>
       </c>
       <c r="B320" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C320" s="7" t="s">
         <v>356</v>
@@ -69142,7 +69142,7 @@
         <v>299</v>
       </c>
       <c r="B321" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C321" s="7" t="s">
         <v>334</v>
@@ -69351,7 +69351,7 @@
         <v>299</v>
       </c>
       <c r="B322" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C322" s="7" t="s">
         <v>334</v>
@@ -69560,7 +69560,7 @@
         <v>299</v>
       </c>
       <c r="B323" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C323" s="7" t="s">
         <v>325</v>
@@ -69769,7 +69769,7 @@
         <v>299</v>
       </c>
       <c r="B324" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C324" s="7" t="s">
         <v>325</v>
@@ -69978,7 +69978,7 @@
         <v>299</v>
       </c>
       <c r="B325" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C325" s="7" t="s">
         <v>325</v>
@@ -70187,7 +70187,7 @@
         <v>299</v>
       </c>
       <c r="B326" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C326" s="7" t="s">
         <v>368</v>
@@ -70396,7 +70396,7 @@
         <v>299</v>
       </c>
       <c r="B327" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C327" s="7" t="s">
         <v>368</v>
@@ -70605,7 +70605,7 @@
         <v>299</v>
       </c>
       <c r="B328" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C328" s="7" t="s">
         <v>368</v>
@@ -70814,7 +70814,7 @@
         <v>299</v>
       </c>
       <c r="B329" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C329" s="7" t="s">
         <v>368</v>
@@ -71023,7 +71023,7 @@
         <v>299</v>
       </c>
       <c r="B330" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C330" s="7" t="s">
         <v>368</v>
@@ -71232,7 +71232,7 @@
         <v>299</v>
       </c>
       <c r="B331" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C331" s="7" t="s">
         <v>368</v>
@@ -71441,7 +71441,7 @@
         <v>299</v>
       </c>
       <c r="B332" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C332" s="7" t="s">
         <v>368</v>
@@ -71650,7 +71650,7 @@
         <v>299</v>
       </c>
       <c r="B333" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C333" s="7" t="s">
         <v>368</v>
@@ -71859,7 +71859,7 @@
         <v>299</v>
       </c>
       <c r="B334" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C334" s="7" t="s">
         <v>368</v>
@@ -72068,7 +72068,7 @@
         <v>299</v>
       </c>
       <c r="B335" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C335" s="7" t="s">
         <v>368</v>
@@ -72277,7 +72277,7 @@
         <v>131</v>
       </c>
       <c r="B336" s="23" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C336" s="17" t="s">
         <v>368</v>
@@ -72486,7 +72486,7 @@
         <v>299</v>
       </c>
       <c r="B337" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C337" s="7" t="s">
         <v>368</v>
@@ -72695,7 +72695,7 @@
         <v>299</v>
       </c>
       <c r="B338" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C338" s="7" t="s">
         <v>368</v>
@@ -72904,7 +72904,7 @@
         <v>69</v>
       </c>
       <c r="B339" s="23" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C339" s="7" t="s">
         <v>368</v>
@@ -73113,7 +73113,7 @@
         <v>69</v>
       </c>
       <c r="B340" s="23" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C340" s="7" t="s">
         <v>368</v>
@@ -73322,7 +73322,7 @@
         <v>69</v>
       </c>
       <c r="B341" s="23" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C341" s="7" t="s">
         <v>368</v>
@@ -73531,7 +73531,7 @@
         <v>69</v>
       </c>
       <c r="B342" s="23" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C342" s="7" t="s">
         <v>368</v>

</xml_diff>